<commit_message>
adding Atezo + Pembro and also fixing Herceptin error
</commit_message>
<xml_diff>
--- a/data/Bx_Herceptin.xlsx
+++ b/data/Bx_Herceptin.xlsx
@@ -9,36 +9,38 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10180" yWindow="460" windowWidth="24700" windowHeight="16840" tabRatio="500"/>
+    <workbookView xWindow="1960" yWindow="460" windowWidth="24700" windowHeight="16840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ABCdrug">Sheet1!$F$36</definedName>
-    <definedName name="ABCsol">Sheet1!$F$37</definedName>
+    <definedName name="ABCdrug">Sheet1!$F$38</definedName>
+    <definedName name="ABCsol">Sheet1!$F$39</definedName>
     <definedName name="CL">Sheet1!$F$4</definedName>
-    <definedName name="eps">Sheet1!$F$41</definedName>
+    <definedName name="eps">Sheet1!$F$43</definedName>
     <definedName name="k12D">Sheet1!$F$11</definedName>
-    <definedName name="k13D">Sheet1!$F$42</definedName>
-    <definedName name="k13DS">Sheet1!$F$44</definedName>
-    <definedName name="k13S">Sheet1!$F$43</definedName>
+    <definedName name="k13D">Sheet1!$F$44</definedName>
+    <definedName name="k13DS">Sheet1!$F$46</definedName>
+    <definedName name="k13S">Sheet1!$F$45</definedName>
     <definedName name="k21D">Sheet1!$F$12</definedName>
-    <definedName name="Kd">Sheet1!$F$14</definedName>
+    <definedName name="Kd">Sheet1!$F$16</definedName>
     <definedName name="keD">Sheet1!$F$5</definedName>
-    <definedName name="koff">Sheet1!$F$14</definedName>
-    <definedName name="kshed">Sheet1!$F$26</definedName>
-    <definedName name="P">Sheet1!$F$38</definedName>
+    <definedName name="keT3_">Sheet1!$F$36</definedName>
+    <definedName name="koff">Sheet1!$F$16</definedName>
+    <definedName name="kshed">Sheet1!$F$28</definedName>
+    <definedName name="P">Sheet1!$F$40</definedName>
     <definedName name="Q">Sheet1!$F$6</definedName>
-    <definedName name="Rcap">Sheet1!$F$39</definedName>
-    <definedName name="Rkrogh">Sheet1!$F$40</definedName>
+    <definedName name="Rcap">Sheet1!$F$41</definedName>
+    <definedName name="Rkrogh">Sheet1!$F$42</definedName>
+    <definedName name="T30_">Sheet1!$F$25</definedName>
     <definedName name="Vc">Sheet1!$F$7</definedName>
     <definedName name="VcDS">Sheet1!$F$10</definedName>
     <definedName name="VcS">Sheet1!$F$9</definedName>
     <definedName name="Vp">Sheet1!$F$8</definedName>
-    <definedName name="Vtum">Sheet1!$F$28</definedName>
-    <definedName name="VtumDS">Sheet1!$F$30</definedName>
-    <definedName name="VtumS">Sheet1!$F$29</definedName>
+    <definedName name="Vtum">Sheet1!$F$30</definedName>
+    <definedName name="VtumDS">Sheet1!$F$32</definedName>
+    <definedName name="VtumS">Sheet1!$F$31</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -53,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="120">
   <si>
     <t>Parameter</t>
   </si>
@@ -169,21 +171,6 @@
     <t>ksynS3</t>
   </si>
   <si>
-    <t>ksynM3</t>
-  </si>
-  <si>
-    <t>kshedM3</t>
-  </si>
-  <si>
-    <t>kshedDM3</t>
-  </si>
-  <si>
-    <t>keM3</t>
-  </si>
-  <si>
-    <t>keDM3</t>
-  </si>
-  <si>
     <t>Comment or Reference</t>
   </si>
   <si>
@@ -364,15 +351,9 @@
     <t>NA</t>
   </si>
   <si>
-    <t>ksynM1</t>
-  </si>
-  <si>
     <t>Cilliers16</t>
   </si>
   <si>
-    <t>M30</t>
-  </si>
-  <si>
     <t>Initial Concentration</t>
   </si>
   <si>
@@ -401,6 +382,39 @@
   </si>
   <si>
     <t>equal to k13D</t>
+  </si>
+  <si>
+    <t>ksynT1</t>
+  </si>
+  <si>
+    <t>T30</t>
+  </si>
+  <si>
+    <t>ksynT3</t>
+  </si>
+  <si>
+    <t>kshedT3</t>
+  </si>
+  <si>
+    <t>kshedDT3</t>
+  </si>
+  <si>
+    <t>keT3</t>
+  </si>
+  <si>
+    <t>keDT3</t>
+  </si>
+  <si>
+    <t>Membrane-Bound Target</t>
+  </si>
+  <si>
+    <t>MWD</t>
+  </si>
+  <si>
+    <t>MWT</t>
+  </si>
+  <si>
+    <t>google search</t>
   </si>
 </sst>
 </file>
@@ -918,10 +932,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -943,13 +957,13 @@
         <v>8</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -961,13 +975,13 @@
         <v>1</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -975,13 +989,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>5</v>
@@ -1002,13 +1016,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>7</v>
@@ -1029,28 +1043,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F4" s="6">
         <v>0.22</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -1058,13 +1072,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>13</v>
@@ -1077,7 +1091,7 @@
         <v>4</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="I5" s="12"/>
     </row>
@@ -1086,28 +1100,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F6" s="6">
         <v>0.36</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -1115,13 +1129,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>21</v>
@@ -1133,10 +1147,10 @@
         <v>2</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -1144,13 +1158,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>22</v>
@@ -1162,10 +1176,10 @@
         <v>2</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -1173,25 +1187,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>2</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="I9" s="12"/>
     </row>
@@ -1200,25 +1214,25 @@
         <v>9</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>2</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="I10" s="12"/>
     </row>
@@ -1227,13 +1241,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>9</v>
@@ -1246,7 +1260,7 @@
         <v>4</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="I11" s="12"/>
     </row>
@@ -1255,13 +1269,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>10</v>
@@ -1274,576 +1288,573 @@
         <v>4</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="I12" s="12"/>
     </row>
     <row r="13" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15"/>
-      <c r="B13" s="15" t="s">
-        <v>51</v>
-      </c>
+      <c r="B13" s="15"/>
       <c r="C13" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" s="6">
+        <v>145</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F14" s="6">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="15"/>
+      <c r="B15" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="H15" s="5"/>
+      <c r="I15" s="16"/>
+    </row>
+    <row r="16" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="11">
+        <v>12</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I16" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="11">
+        <v>13</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="D13" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="H13" s="5"/>
-      <c r="I13" s="16"/>
-    </row>
-    <row r="14" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="11">
-        <v>12</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="I14" s="16" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="11">
-        <v>13</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="E15" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F17" s="6">
         <f>0.00035*60*60*24</f>
         <v>30.240000000000002</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G17" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="I15" s="16" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="15">
+      <c r="H17" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I17" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="15">
         <v>14</v>
       </c>
-      <c r="B16" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="E16" s="5" t="s">
+      <c r="B18" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F18" s="6">
         <f>0.00035*60*60*24</f>
         <v>30.240000000000002</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H16" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="I16" s="16" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="15">
+      <c r="H18" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I18" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="15">
         <v>15</v>
       </c>
-      <c r="B17" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="E17" s="5" t="s">
+      <c r="B19" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="6">
-        <f>F15/F14</f>
+      <c r="F19" s="6">
+        <f>F17/F16</f>
         <v>60.480000000000004</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H17" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="I17" s="16" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="15">
+      <c r="H19" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="15">
         <v>16</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="E18" s="5" t="s">
+      <c r="B20" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="6">
-        <f>F17</f>
+      <c r="F20" s="6">
+        <f>F19</f>
         <v>60.480000000000004</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G20" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="I18" s="16" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="11">
+      <c r="H20" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="11">
         <v>17</v>
       </c>
-      <c r="B19" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="E19" s="5" t="s">
+      <c r="B21" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="G19" s="5" t="s">
+      <c r="F21" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H19" s="5">
+      <c r="H21" s="5">
         <v>0</v>
       </c>
-      <c r="I19" s="16"/>
-    </row>
-    <row r="20" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="11">
-        <v>18</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I20" s="12"/>
-    </row>
-    <row r="21" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="11">
-        <v>19</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H21" s="4">
-        <v>0</v>
-      </c>
-      <c r="I21" s="12"/>
+      <c r="I21" s="16"/>
     </row>
     <row r="22" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
+        <v>18</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I22" s="12"/>
+    </row>
+    <row r="23" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="11">
+        <v>19</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H23" s="4">
+        <v>0</v>
+      </c>
+      <c r="I23" s="12"/>
+    </row>
+    <row r="24" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="11">
         <v>20</v>
       </c>
-      <c r="B22" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E22" s="4" t="s">
+      <c r="B24" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F22" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="G22" s="4" t="s">
+      <c r="F24" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G24" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H22" s="4">
+      <c r="H24" s="4">
         <v>0</v>
       </c>
-      <c r="I22" s="12"/>
-    </row>
-    <row r="23" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="15">
+      <c r="I24" s="12"/>
+    </row>
+    <row r="25" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="15">
         <v>20.100000000000001</v>
       </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="F23" s="6">
+      <c r="B25" s="15"/>
+      <c r="C25" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F25" s="6">
         <v>830</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G25" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I25" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="15">
+        <v>20.2</v>
+      </c>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F26" s="6">
+        <v>0</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="I26" s="16"/>
+    </row>
+    <row r="27" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="11">
+        <v>21</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F27" s="7">
+        <f>T30_*keT3_</f>
+        <v>2366.4960000000001</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H27" s="4">
+        <v>1</v>
+      </c>
+      <c r="I27" s="19"/>
+    </row>
+    <row r="28" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="11">
+        <v>22</v>
+      </c>
+      <c r="B28" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="H23" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="I23" s="16" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="15">
-        <v>20.2</v>
-      </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F24" s="6">
-        <v>0</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="I24" s="16"/>
-    </row>
-    <row r="25" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="15">
-        <v>21</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F25" s="6">
-        <v>10</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H25" s="5">
-        <v>1</v>
-      </c>
-      <c r="I25" s="19"/>
-    </row>
-    <row r="26" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="11">
-        <v>22</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="G26" s="5" t="s">
+      <c r="C28" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G28" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H26" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="I26" s="16"/>
-    </row>
-    <row r="27" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="11">
-        <v>23</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I27" s="12"/>
-    </row>
-    <row r="28" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="11">
-        <v>24</v>
-      </c>
-      <c r="B28" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="D28" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F28" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I28" s="21"/>
+      <c r="H28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I28" s="16"/>
     </row>
     <row r="29" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>25</v>
+        <v>113</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G29" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I29" s="12"/>
+    </row>
+    <row r="30" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="11">
+        <v>24</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F30" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H29" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I29" s="12"/>
-    </row>
-    <row r="30" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="11">
-        <v>26</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I30" s="12"/>
+      <c r="H30" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I30" s="21"/>
     </row>
     <row r="31" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F31" s="7">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>97</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H31" s="4">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="I31" s="12"/>
     </row>
     <row r="32" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H32" s="4">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="I32" s="12"/>
     </row>
     <row r="33" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>102</v>
+        <v>14</v>
+      </c>
+      <c r="F33" s="7">
+        <v>0</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>4</v>
@@ -1854,366 +1865,420 @@
       <c r="I33" s="12"/>
     </row>
     <row r="34" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="15">
+      <c r="A34" s="11">
+        <v>28</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H34" s="4">
+        <v>0</v>
+      </c>
+      <c r="I34" s="12"/>
+    </row>
+    <row r="35" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="11">
+        <v>29</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H35" s="4">
+        <v>0</v>
+      </c>
+      <c r="I35" s="12"/>
+    </row>
+    <row r="36" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="15">
         <v>30</v>
       </c>
-      <c r="B34" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F34" s="6">
+      <c r="B36" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F36" s="6">
         <f>0.000033*60*60*24</f>
         <v>2.8512</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="G36" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H34" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="I34" s="16" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="15">
+      <c r="H36" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I36" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="15">
         <v>31</v>
       </c>
-      <c r="B35" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F35" s="6">
+      <c r="B37" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F37" s="6">
         <f>0.000033*60*60*24</f>
         <v>2.8512</v>
       </c>
-      <c r="G35" s="5" t="s">
+      <c r="G37" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H35" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="I35" s="16" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="11">
-        <v>32</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="11">
-        <v>33</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>59</v>
+      <c r="H37" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I37" s="16" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="11">
+        <v>32</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="11">
+        <v>33</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="11">
         <v>33.1</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F38" s="22">
+      <c r="E40" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F40" s="22">
         <f>0.000000003*1000000*60*60*24</f>
         <v>259.2</v>
       </c>
-      <c r="G38" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="I38" s="14" t="s">
+      <c r="G40" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I40" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="11">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F41" s="6">
+        <v>8</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I41" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="11">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="11">
-        <v>33.200000000000003</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F39" s="6">
-        <v>8</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="I39" s="14" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="11">
-        <v>33.299999999999997</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F40" s="6">
+      <c r="F42" s="6">
         <v>75</v>
       </c>
-      <c r="G40" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="I40" s="14" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="11"/>
-      <c r="E41" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F41" s="6">
+      <c r="G42" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I42" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="11"/>
+      <c r="E43" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F43" s="6">
         <v>0.24</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I41" s="14" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="11">
+      <c r="I43" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="11">
         <v>34</v>
       </c>
-      <c r="B42" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="E42" s="4" t="s">
+      <c r="B44" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="E44" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F42" s="7">
+      <c r="F44" s="7">
         <f>2*P*Rcap/Rkrogh^2</f>
         <v>0.73727999999999994</v>
       </c>
-      <c r="G42" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I42" s="12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="11">
-        <v>35</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H43" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I43" s="12"/>
-    </row>
-    <row r="44" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="11">
-        <v>36</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>102</v>
-      </c>
       <c r="G44" s="4" t="s">
         <v>4</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I44" s="12"/>
+        <v>51</v>
+      </c>
+      <c r="I44" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="45" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="11">
+        <v>35</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I45" s="12"/>
+    </row>
+    <row r="46" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="11">
+        <v>36</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I46" s="12"/>
+    </row>
+    <row r="47" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="11">
         <v>37</v>
       </c>
-      <c r="B45" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E45" s="4" t="s">
+      <c r="B47" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E47" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F45" s="7">
+      <c r="F47" s="7">
         <f>k13D</f>
         <v>0.73727999999999994</v>
       </c>
-      <c r="G45" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H45" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I45" s="12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="11">
-        <v>38</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H46" s="11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="11">
-        <v>39</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C47" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D47" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>102</v>
-      </c>
       <c r="G47" s="4" t="s">
         <v>4</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I47" s="12"/>
+        <v>51</v>
+      </c>
+      <c r="I47" s="12" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="48" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="H48" s="11"/>
-    </row>
-    <row r="49" spans="6:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="H49" s="4"/>
+      <c r="A48" s="11">
+        <v>38</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H48" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="11">
+        <v>39</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="I49" s="12"/>
     </row>
-    <row r="54" spans="6:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="F54" s="12"/>
-      <c r="H54" s="11"/>
+    <row r="50" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H50" s="11"/>
+    </row>
+    <row r="51" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H51" s="4"/>
+      <c r="I51" s="12"/>
+    </row>
+    <row r="56" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F56" s="12"/>
+      <c r="H56" s="11"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F271">
+  <conditionalFormatting sqref="F273">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="derived">
-      <formula>NOT(ISERROR(SEARCH("derived",F271)))</formula>
+      <formula>NOT(ISERROR(SEARCH("derived",F273)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>